<commit_message>
Uren Registratie vorige week en 2-11-15
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="73">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -240,6 +241,9 @@
   </si>
   <si>
     <t>Michiel te laat : Sven te laat</t>
+  </si>
+  <si>
+    <t>Michiel Ziek : Fahrettin ziek? : Roos te laat</t>
   </si>
 </sst>
 </file>
@@ -836,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,15 +920,15 @@
       <c r="L2" s="1"/>
       <c r="M2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="N2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="O2" s="23">
         <f>N2/M2</f>
-        <v>0.77058823529411768</v>
+        <v>0.75690607734806625</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>0</v>
@@ -960,11 +964,11 @@
       <c r="M3" s="12"/>
       <c r="N3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="O3" s="23">
         <f>N3/M2</f>
-        <v>0.69411764705882351</v>
+        <v>0.68508287292817682</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>1</v>
@@ -1000,11 +1004,11 @@
       <c r="M4" s="12"/>
       <c r="N4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="O4" s="23">
         <f>N4/M2</f>
-        <v>0.92352941176470593</v>
+        <v>0.92817679558011046</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>2</v>
@@ -1040,11 +1044,11 @@
       <c r="M5" s="12"/>
       <c r="N5" s="7">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="O5" s="23">
         <f>N5/M2</f>
-        <v>0.55882352941176472</v>
+        <v>0.58563535911602205</v>
       </c>
       <c r="P5" s="17" t="s">
         <v>3</v>
@@ -1080,11 +1084,11 @@
       <c r="M6" s="12"/>
       <c r="N6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="O6" s="23">
         <f>N6/M2</f>
-        <v>0.95882352941176474</v>
+        <v>0.95580110497237569</v>
       </c>
       <c r="P6" s="18" t="s">
         <v>4</v>
@@ -1122,11 +1126,11 @@
       <c r="M7" s="12"/>
       <c r="N7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="O7" s="23">
         <f>N7/M2</f>
-        <v>0.91764705882352937</v>
+        <v>0.92265193370165743</v>
       </c>
       <c r="P7" s="19" t="s">
         <v>5</v>
@@ -1764,7 +1768,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="11">
-        <f t="shared" ref="C32:G32" si="3">SUM(C27:C31)</f>
+        <f t="shared" ref="C32:H32" si="3">SUM(C27:C31)</f>
         <v>16</v>
       </c>
       <c r="D32" s="11">
@@ -1784,7 +1788,7 @@
         <v>18</v>
       </c>
       <c r="H32" s="11">
-        <f>SUM(H27:H31)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="I32" s="11"/>
@@ -2850,6 +2854,24 @@
         <v>12</v>
       </c>
       <c r="B78" s="12"/>
+      <c r="C78" s="13">
+        <v>2</v>
+      </c>
+      <c r="D78" s="13">
+        <v>2</v>
+      </c>
+      <c r="E78" s="13">
+        <v>2</v>
+      </c>
+      <c r="F78" s="13">
+        <v>2</v>
+      </c>
+      <c r="G78" s="13">
+        <v>2</v>
+      </c>
+      <c r="H78" s="13">
+        <v>2</v>
+      </c>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
       <c r="K78" s="12"/>
@@ -2861,12 +2883,24 @@
         <v>13</v>
       </c>
       <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
+      <c r="C79" s="25">
+        <v>4</v>
+      </c>
+      <c r="D79" s="25">
+        <v>4</v>
+      </c>
+      <c r="E79" s="25">
+        <v>4</v>
+      </c>
+      <c r="F79" s="25">
+        <v>4</v>
+      </c>
+      <c r="G79" s="25">
+        <v>4</v>
+      </c>
+      <c r="H79" s="25">
+        <v>4</v>
+      </c>
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
       <c r="K79" s="11"/>
@@ -2878,31 +2912,31 @@
         <v>15</v>
       </c>
       <c r="B80" s="11">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C80" s="11">
         <f t="shared" ref="C80:H80" si="9">SUM(C75:C79)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D80" s="11">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E80" s="11">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F80" s="11">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G80" s="11">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H80" s="11">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I80" s="11"/>
       <c r="J80" s="11"/>
@@ -2933,10 +2967,30 @@
         <v>9</v>
       </c>
       <c r="B83" s="12"/>
+      <c r="C83" s="14">
+        <v>0</v>
+      </c>
+      <c r="D83" s="14">
+        <v>0</v>
+      </c>
+      <c r="E83" s="13">
+        <v>5</v>
+      </c>
+      <c r="F83" s="13">
+        <v>5</v>
+      </c>
+      <c r="G83" s="24">
+        <v>4</v>
+      </c>
+      <c r="H83" s="13">
+        <v>5</v>
+      </c>
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
-      <c r="L83" s="2"/>
+      <c r="L83" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="M83" s="12"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
@@ -2994,7 +3048,7 @@
         <v>15</v>
       </c>
       <c r="B88" s="11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C88" s="11">
         <f t="shared" ref="C88:H88" si="10">SUM(C83:C87)</f>
@@ -3006,19 +3060,19 @@
       </c>
       <c r="E88" s="11">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F88" s="11">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G88" s="11">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H88" s="11">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I88" s="11"/>
       <c r="J88" s="11"/>

</xml_diff>

<commit_message>
Aseet Lisr Vakanties Toegevoegd
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riefo\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\1. Game-Lab 1\8. GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>Rief Ziek : Roos 2 lesuren eerder naar huis</t>
   </si>
   <si>
-    <t>Week 4:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rief Ziek </t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Michiel Ziek : Fahrettin te laat : Sven te laat</t>
+  </si>
+  <si>
+    <t>Week 53:</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -557,6 +557,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -842,26 +857,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="8" width="10.88671875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="7"/>
-    <col min="12" max="12" width="59.109375" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" style="23" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="8" width="10.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="7"/>
+    <col min="12" max="12" width="59.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="23" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
@@ -905,7 +920,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -936,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -976,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1138,7 +1153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1175,10 +1190,10 @@
       <c r="L8" s="29"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L9" s="30"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +1210,7 @@
       <c r="L10" s="31"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1226,7 +1241,7 @@
       </c>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1255,7 +1270,7 @@
       <c r="L12" s="32"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1286,7 +1301,7 @@
       </c>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1315,7 +1330,7 @@
       <c r="L14" s="32"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +1361,7 @@
       </c>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -1383,10 +1398,10 @@
       <c r="L16" s="29"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L17" s="30"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1403,7 +1418,7 @@
       <c r="L18" s="31"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1432,7 +1447,7 @@
       <c r="L19" s="32"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1463,7 +1478,7 @@
       </c>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1494,7 +1509,7 @@
       </c>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1523,7 +1538,7 @@
       <c r="L22" s="32"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1569,7 @@
       </c>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
@@ -1591,8 +1606,8 @@
       <c r="L24" s="3"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
@@ -1609,7 +1624,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1653,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1669,7 +1684,7 @@
       </c>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1696,11 +1711,11 @@
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M29" s="12"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1727,11 +1742,11 @@
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M30" s="12"/>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
@@ -1762,7 +1777,7 @@
       </c>
       <c r="M31" s="12"/>
     </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
@@ -1799,8 +1814,8 @@
       <c r="L32" s="3"/>
       <c r="M32" s="12"/>
     </row>
-    <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>22</v>
       </c>
@@ -1817,7 +1832,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="12"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>9</v>
       </c>
@@ -1848,7 +1863,7 @@
       </c>
       <c r="M35" s="12"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -1879,7 +1894,7 @@
       </c>
       <c r="M36" s="12"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
@@ -1910,7 +1925,7 @@
       </c>
       <c r="M37" s="12"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
@@ -1937,11 +1952,11 @@
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M38" s="12"/>
     </row>
-    <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>13</v>
       </c>
@@ -1968,11 +1983,11 @@
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
       <c r="L39" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M39" s="12"/>
     </row>
-    <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>15</v>
       </c>
@@ -2009,8 +2024,8 @@
       <c r="L40" s="3"/>
       <c r="M40" s="12"/>
     </row>
-    <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
@@ -2027,7 +2042,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="12"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
@@ -2054,11 +2069,11 @@
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M43" s="12"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>10</v>
       </c>
@@ -2085,11 +2100,11 @@
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M44" s="12"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
@@ -2118,7 +2133,7 @@
       <c r="L45" s="2"/>
       <c r="M45" s="12"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2145,11 +2160,11 @@
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M46" s="12"/>
     </row>
-    <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>13</v>
       </c>
@@ -2176,11 +2191,11 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
       <c r="L47" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M47" s="12"/>
     </row>
-    <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>15</v>
       </c>
@@ -2217,8 +2232,8 @@
       <c r="L48" s="3"/>
       <c r="M48" s="12"/>
     </row>
-    <row r="49" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
@@ -2235,7 +2250,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="12"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>9</v>
       </c>
@@ -2262,11 +2277,11 @@
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M51" s="12"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>10</v>
       </c>
@@ -2293,11 +2308,11 @@
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M52" s="12"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>11</v>
       </c>
@@ -2324,11 +2339,11 @@
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M53" s="12"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
@@ -2357,7 +2372,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="12"/>
     </row>
-    <row r="55" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2401,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="12"/>
     </row>
-    <row r="56" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>15</v>
       </c>
@@ -2423,8 +2438,8 @@
       <c r="L56" s="3"/>
       <c r="M56" s="12"/>
     </row>
-    <row r="57" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>25</v>
       </c>
@@ -2441,7 +2456,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="12"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>9</v>
       </c>
@@ -2468,11 +2483,11 @@
       <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M59" s="12"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>10</v>
       </c>
@@ -2499,11 +2514,11 @@
       <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M60" s="12"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>11</v>
       </c>
@@ -2530,11 +2545,11 @@
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M61" s="12"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>12</v>
       </c>
@@ -2561,11 +2576,11 @@
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M62" s="12"/>
     </row>
-    <row r="63" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>13</v>
       </c>
@@ -2594,7 +2609,7 @@
       <c r="L63" s="3"/>
       <c r="M63" s="12"/>
     </row>
-    <row r="64" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>15</v>
       </c>
@@ -2631,99 +2646,110 @@
       <c r="L64" s="3"/>
       <c r="M64" s="12"/>
     </row>
-    <row r="65" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="1"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="34"/>
+      <c r="L66" s="35"/>
       <c r="M66" s="12"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="2"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="38"/>
       <c r="M67" s="12"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="2"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="38"/>
       <c r="M68" s="12"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="12"/>
-      <c r="K69" s="12"/>
-      <c r="L69" s="2"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="38"/>
       <c r="M69" s="12"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="12"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
-      <c r="K70" s="12"/>
-      <c r="L70" s="2"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="38"/>
       <c r="M70" s="12"/>
     </row>
-    <row r="71" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="6" t="s">
+    <row r="71" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="3"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="40"/>
+      <c r="H71" s="40"/>
+      <c r="I71" s="40"/>
+      <c r="J71" s="40"/>
+      <c r="K71" s="40"/>
+      <c r="L71" s="41"/>
       <c r="M71" s="12"/>
     </row>
-    <row r="72" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>15</v>
       </c>
@@ -2760,8 +2786,8 @@
       <c r="L72" s="3"/>
       <c r="M72" s="12"/>
     </row>
-    <row r="73" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>27</v>
       </c>
@@ -2778,7 +2804,7 @@
       <c r="L74" s="1"/>
       <c r="M74" s="12"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>9</v>
       </c>
@@ -2789,7 +2815,7 @@
       <c r="L75" s="2"/>
       <c r="M75" s="12"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>10</v>
       </c>
@@ -2816,11 +2842,11 @@
       <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M76" s="12"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>11</v>
       </c>
@@ -2847,11 +2873,11 @@
       <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M77" s="12"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>12</v>
       </c>
@@ -2880,7 +2906,7 @@
       <c r="L78" s="2"/>
       <c r="M78" s="12"/>
     </row>
-    <row r="79" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>13</v>
       </c>
@@ -2909,7 +2935,7 @@
       <c r="L79" s="3"/>
       <c r="M79" s="12"/>
     </row>
-    <row r="80" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>15</v>
       </c>
@@ -2946,8 +2972,8 @@
       <c r="L80" s="3"/>
       <c r="M80" s="12"/>
     </row>
-    <row r="81" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>28</v>
       </c>
@@ -2964,7 +2990,7 @@
       <c r="L82" s="1"/>
       <c r="M82" s="12"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>9</v>
       </c>
@@ -2991,11 +3017,11 @@
       <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M83" s="12"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>10</v>
       </c>
@@ -3026,7 +3052,7 @@
       </c>
       <c r="M84" s="12"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>11</v>
       </c>
@@ -3053,11 +3079,11 @@
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M85" s="12"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>12</v>
       </c>
@@ -3068,7 +3094,7 @@
       <c r="L86" s="2"/>
       <c r="M86" s="12"/>
     </row>
-    <row r="87" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>13</v>
       </c>
@@ -3085,7 +3111,7 @@
       <c r="L87" s="3"/>
       <c r="M87" s="12"/>
     </row>
-    <row r="88" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>15</v>
       </c>
@@ -3122,8 +3148,8 @@
       <c r="L88" s="3"/>
       <c r="M88" s="12"/>
     </row>
-    <row r="89" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>29</v>
       </c>
@@ -3140,7 +3166,7 @@
       <c r="L90" s="1"/>
       <c r="M90" s="12"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>9</v>
       </c>
@@ -3151,7 +3177,7 @@
       <c r="L91" s="2"/>
       <c r="M91" s="12"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>10</v>
       </c>
@@ -3162,7 +3188,7 @@
       <c r="L92" s="2"/>
       <c r="M92" s="12"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>11</v>
       </c>
@@ -3173,7 +3199,7 @@
       <c r="L93" s="2"/>
       <c r="M93" s="12"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>12</v>
       </c>
@@ -3184,7 +3210,7 @@
       <c r="L94" s="2"/>
       <c r="M94" s="12"/>
     </row>
-    <row r="95" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>13</v>
       </c>
@@ -3201,7 +3227,7 @@
       <c r="L95" s="3"/>
       <c r="M95" s="12"/>
     </row>
-    <row r="96" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>15</v>
       </c>
@@ -3238,8 +3264,8 @@
       <c r="L96" s="3"/>
       <c r="M96" s="12"/>
     </row>
-    <row r="97" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>30</v>
       </c>
@@ -3256,7 +3282,7 @@
       <c r="L98" s="1"/>
       <c r="M98" s="12"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>9</v>
       </c>
@@ -3267,7 +3293,7 @@
       <c r="L99" s="2"/>
       <c r="M99" s="12"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>10</v>
       </c>
@@ -3278,7 +3304,7 @@
       <c r="L100" s="2"/>
       <c r="M100" s="12"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>11</v>
       </c>
@@ -3289,7 +3315,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="12"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>12</v>
       </c>
@@ -3300,7 +3326,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="12"/>
     </row>
-    <row r="103" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>13</v>
       </c>
@@ -3317,7 +3343,7 @@
       <c r="L103" s="3"/>
       <c r="M103" s="12"/>
     </row>
-    <row r="104" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>15</v>
       </c>
@@ -3354,8 +3380,8 @@
       <c r="L104" s="3"/>
       <c r="M104" s="12"/>
     </row>
-    <row r="105" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>31</v>
       </c>
@@ -3372,7 +3398,7 @@
       <c r="L106" s="1"/>
       <c r="M106" s="12"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>9</v>
       </c>
@@ -3383,7 +3409,7 @@
       <c r="L107" s="2"/>
       <c r="M107" s="12"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>10</v>
       </c>
@@ -3394,7 +3420,7 @@
       <c r="L108" s="2"/>
       <c r="M108" s="12"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>11</v>
       </c>
@@ -3405,7 +3431,7 @@
       <c r="L109" s="2"/>
       <c r="M109" s="12"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>12</v>
       </c>
@@ -3416,7 +3442,7 @@
       <c r="L110" s="2"/>
       <c r="M110" s="12"/>
     </row>
-    <row r="111" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>13</v>
       </c>
@@ -3433,7 +3459,7 @@
       <c r="L111" s="3"/>
       <c r="M111" s="12"/>
     </row>
-    <row r="112" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>15</v>
       </c>
@@ -3470,8 +3496,8 @@
       <c r="L112" s="3"/>
       <c r="M112" s="12"/>
     </row>
-    <row r="113" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>32</v>
       </c>
@@ -3488,7 +3514,7 @@
       <c r="L114" s="1"/>
       <c r="M114" s="12"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>9</v>
       </c>
@@ -3499,7 +3525,7 @@
       <c r="L115" s="2"/>
       <c r="M115" s="12"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>10</v>
       </c>
@@ -3510,7 +3536,7 @@
       <c r="L116" s="2"/>
       <c r="M116" s="12"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>11</v>
       </c>
@@ -3521,7 +3547,7 @@
       <c r="L117" s="2"/>
       <c r="M117" s="12"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>12</v>
       </c>
@@ -3532,7 +3558,7 @@
       <c r="L118" s="2"/>
       <c r="M118" s="12"/>
     </row>
-    <row r="119" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>13</v>
       </c>
@@ -3549,7 +3575,7 @@
       <c r="L119" s="3"/>
       <c r="M119" s="12"/>
     </row>
-    <row r="120" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>15</v>
       </c>
@@ -3586,8 +3612,8 @@
       <c r="L120" s="3"/>
       <c r="M120" s="12"/>
     </row>
-    <row r="121" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>33</v>
       </c>
@@ -3604,7 +3630,7 @@
       <c r="L122" s="1"/>
       <c r="M122" s="12"/>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>9</v>
       </c>
@@ -3615,7 +3641,7 @@
       <c r="L123" s="2"/>
       <c r="M123" s="12"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>10</v>
       </c>
@@ -3626,7 +3652,7 @@
       <c r="L124" s="2"/>
       <c r="M124" s="12"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>11</v>
       </c>
@@ -3637,7 +3663,7 @@
       <c r="L125" s="2"/>
       <c r="M125" s="12"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>12</v>
       </c>
@@ -3648,7 +3674,7 @@
       <c r="L126" s="2"/>
       <c r="M126" s="12"/>
     </row>
-    <row r="127" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>13</v>
       </c>
@@ -3665,7 +3691,7 @@
       <c r="L127" s="3"/>
       <c r="M127" s="12"/>
     </row>
-    <row r="128" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>15</v>
       </c>
@@ -3702,8 +3728,8 @@
       <c r="L128" s="3"/>
       <c r="M128" s="12"/>
     </row>
-    <row r="129" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>34</v>
       </c>
@@ -3720,7 +3746,7 @@
       <c r="L130" s="1"/>
       <c r="M130" s="12"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +3757,7 @@
       <c r="L131" s="2"/>
       <c r="M131" s="12"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>10</v>
       </c>
@@ -3742,7 +3768,7 @@
       <c r="L132" s="2"/>
       <c r="M132" s="12"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>11</v>
       </c>
@@ -3753,7 +3779,7 @@
       <c r="L133" s="2"/>
       <c r="M133" s="12"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>12</v>
       </c>
@@ -3764,7 +3790,7 @@
       <c r="L134" s="2"/>
       <c r="M134" s="12"/>
     </row>
-    <row r="135" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>13</v>
       </c>
@@ -3781,7 +3807,7 @@
       <c r="L135" s="3"/>
       <c r="M135" s="12"/>
     </row>
-    <row r="136" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>15</v>
       </c>
@@ -3818,86 +3844,110 @@
       <c r="L136" s="3"/>
       <c r="M136" s="12"/>
     </row>
-    <row r="137" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A138" s="4" t="s">
+    <row r="137" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A138" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B138" s="8"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
-      <c r="F138" s="8"/>
-      <c r="G138" s="8"/>
-      <c r="H138" s="8"/>
-      <c r="I138" s="8"/>
-      <c r="J138" s="8"/>
-      <c r="K138" s="8"/>
-      <c r="L138" s="1"/>
+      <c r="B138" s="34"/>
+      <c r="C138" s="34"/>
+      <c r="D138" s="34"/>
+      <c r="E138" s="34"/>
+      <c r="F138" s="34"/>
+      <c r="G138" s="34"/>
+      <c r="H138" s="34"/>
+      <c r="I138" s="34"/>
+      <c r="J138" s="34"/>
+      <c r="K138" s="34"/>
+      <c r="L138" s="35"/>
       <c r="M138" s="12"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A139" s="5" t="s">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A139" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B139" s="12"/>
-      <c r="I139" s="12"/>
-      <c r="J139" s="12"/>
-      <c r="K139" s="12"/>
-      <c r="L139" s="2"/>
+      <c r="B139" s="37"/>
+      <c r="C139" s="16"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
+      <c r="I139" s="37"/>
+      <c r="J139" s="37"/>
+      <c r="K139" s="37"/>
+      <c r="L139" s="38"/>
       <c r="M139" s="12"/>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A140" s="5" t="s">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A140" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B140" s="12"/>
-      <c r="I140" s="12"/>
-      <c r="J140" s="12"/>
-      <c r="K140" s="12"/>
-      <c r="L140" s="2"/>
+      <c r="B140" s="37"/>
+      <c r="C140" s="16"/>
+      <c r="D140" s="16"/>
+      <c r="E140" s="16"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
+      <c r="I140" s="37"/>
+      <c r="J140" s="37"/>
+      <c r="K140" s="37"/>
+      <c r="L140" s="38"/>
       <c r="M140" s="12"/>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A141" s="5" t="s">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A141" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B141" s="12"/>
-      <c r="I141" s="12"/>
-      <c r="J141" s="12"/>
-      <c r="K141" s="12"/>
-      <c r="L141" s="2"/>
+      <c r="B141" s="37"/>
+      <c r="C141" s="16"/>
+      <c r="D141" s="16"/>
+      <c r="E141" s="16"/>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="16"/>
+      <c r="I141" s="37"/>
+      <c r="J141" s="37"/>
+      <c r="K141" s="37"/>
+      <c r="L141" s="38"/>
       <c r="M141" s="12"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A142" s="5" t="s">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A142" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="12"/>
-      <c r="I142" s="12"/>
-      <c r="J142" s="12"/>
-      <c r="K142" s="12"/>
-      <c r="L142" s="2"/>
+      <c r="B142" s="37"/>
+      <c r="C142" s="16"/>
+      <c r="D142" s="16"/>
+      <c r="E142" s="16"/>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="16"/>
+      <c r="I142" s="37"/>
+      <c r="J142" s="37"/>
+      <c r="K142" s="37"/>
+      <c r="L142" s="38"/>
       <c r="M142" s="12"/>
     </row>
-    <row r="143" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="6" t="s">
+    <row r="143" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
-      <c r="G143" s="11"/>
-      <c r="H143" s="11"/>
-      <c r="I143" s="11"/>
-      <c r="J143" s="11"/>
-      <c r="K143" s="11"/>
-      <c r="L143" s="3"/>
+      <c r="B143" s="40"/>
+      <c r="C143" s="40"/>
+      <c r="D143" s="40"/>
+      <c r="E143" s="40"/>
+      <c r="F143" s="40"/>
+      <c r="G143" s="40"/>
+      <c r="H143" s="40"/>
+      <c r="I143" s="40"/>
+      <c r="J143" s="40"/>
+      <c r="K143" s="40"/>
+      <c r="L143" s="41"/>
       <c r="M143" s="12"/>
     </row>
-    <row r="144" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>15</v>
       </c>
@@ -3934,86 +3984,110 @@
       <c r="L144" s="3"/>
       <c r="M144" s="12"/>
     </row>
-    <row r="145" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B146" s="8"/>
-      <c r="C146" s="8"/>
-      <c r="D146" s="8"/>
-      <c r="E146" s="8"/>
-      <c r="F146" s="8"/>
-      <c r="G146" s="8"/>
-      <c r="H146" s="8"/>
-      <c r="I146" s="8"/>
-      <c r="J146" s="8"/>
-      <c r="K146" s="8"/>
-      <c r="L146" s="1"/>
+    <row r="145" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B146" s="34"/>
+      <c r="C146" s="34"/>
+      <c r="D146" s="34"/>
+      <c r="E146" s="34"/>
+      <c r="F146" s="34"/>
+      <c r="G146" s="34"/>
+      <c r="H146" s="34"/>
+      <c r="I146" s="34"/>
+      <c r="J146" s="34"/>
+      <c r="K146" s="34"/>
+      <c r="L146" s="35"/>
       <c r="M146" s="12"/>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A147" s="5" t="s">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B147" s="12"/>
-      <c r="I147" s="12"/>
-      <c r="J147" s="12"/>
-      <c r="K147" s="12"/>
-      <c r="L147" s="2"/>
+      <c r="B147" s="37"/>
+      <c r="C147" s="16"/>
+      <c r="D147" s="16"/>
+      <c r="E147" s="16"/>
+      <c r="F147" s="16"/>
+      <c r="G147" s="16"/>
+      <c r="H147" s="16"/>
+      <c r="I147" s="37"/>
+      <c r="J147" s="37"/>
+      <c r="K147" s="37"/>
+      <c r="L147" s="38"/>
       <c r="M147" s="12"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A148" s="5" t="s">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B148" s="12"/>
-      <c r="I148" s="12"/>
-      <c r="J148" s="12"/>
-      <c r="K148" s="12"/>
-      <c r="L148" s="2"/>
+      <c r="B148" s="37"/>
+      <c r="C148" s="16"/>
+      <c r="D148" s="16"/>
+      <c r="E148" s="16"/>
+      <c r="F148" s="16"/>
+      <c r="G148" s="16"/>
+      <c r="H148" s="16"/>
+      <c r="I148" s="37"/>
+      <c r="J148" s="37"/>
+      <c r="K148" s="37"/>
+      <c r="L148" s="38"/>
       <c r="M148" s="12"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A149" s="5" t="s">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B149" s="12"/>
-      <c r="I149" s="12"/>
-      <c r="J149" s="12"/>
-      <c r="K149" s="12"/>
-      <c r="L149" s="2"/>
+      <c r="B149" s="37"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="16"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="16"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="16"/>
+      <c r="I149" s="37"/>
+      <c r="J149" s="37"/>
+      <c r="K149" s="37"/>
+      <c r="L149" s="38"/>
       <c r="M149" s="12"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A150" s="5" t="s">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B150" s="12"/>
-      <c r="I150" s="12"/>
-      <c r="J150" s="12"/>
-      <c r="K150" s="12"/>
-      <c r="L150" s="2"/>
+      <c r="B150" s="37"/>
+      <c r="C150" s="16"/>
+      <c r="D150" s="16"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="16"/>
+      <c r="I150" s="37"/>
+      <c r="J150" s="37"/>
+      <c r="K150" s="37"/>
+      <c r="L150" s="38"/>
       <c r="M150" s="12"/>
     </row>
-    <row r="151" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="6" t="s">
+    <row r="151" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
-      <c r="G151" s="11"/>
-      <c r="H151" s="11"/>
-      <c r="I151" s="11"/>
-      <c r="J151" s="11"/>
-      <c r="K151" s="11"/>
-      <c r="L151" s="3"/>
+      <c r="B151" s="40"/>
+      <c r="C151" s="40"/>
+      <c r="D151" s="40"/>
+      <c r="E151" s="40"/>
+      <c r="F151" s="40"/>
+      <c r="G151" s="40"/>
+      <c r="H151" s="40"/>
+      <c r="I151" s="40"/>
+      <c r="J151" s="40"/>
+      <c r="K151" s="40"/>
+      <c r="L151" s="41"/>
       <c r="M151" s="12"/>
     </row>
-    <row r="152" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>15</v>
       </c>
@@ -4050,10 +4124,10 @@
       <c r="L152" s="3"/>
       <c r="M152" s="12"/>
     </row>
-    <row r="153" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
@@ -4068,7 +4142,7 @@
       <c r="L154" s="1"/>
       <c r="M154" s="12"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>9</v>
       </c>
@@ -4079,7 +4153,7 @@
       <c r="L155" s="2"/>
       <c r="M155" s="12"/>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>10</v>
       </c>
@@ -4090,7 +4164,7 @@
       <c r="L156" s="2"/>
       <c r="M156" s="12"/>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>11</v>
       </c>
@@ -4101,7 +4175,7 @@
       <c r="L157" s="2"/>
       <c r="M157" s="12"/>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>12</v>
       </c>
@@ -4112,7 +4186,7 @@
       <c r="L158" s="2"/>
       <c r="M158" s="12"/>
     </row>
-    <row r="159" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>13</v>
       </c>
@@ -4129,7 +4203,7 @@
       <c r="L159" s="3"/>
       <c r="M159" s="12"/>
     </row>
-    <row r="160" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>15</v>
       </c>
@@ -4166,10 +4240,10 @@
       <c r="L160" s="3"/>
       <c r="M160" s="12"/>
     </row>
-    <row r="161" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
@@ -4184,7 +4258,7 @@
       <c r="L162" s="1"/>
       <c r="M162" s="12"/>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>9</v>
       </c>
@@ -4195,7 +4269,7 @@
       <c r="L163" s="2"/>
       <c r="M163" s="12"/>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>10</v>
       </c>
@@ -4206,7 +4280,7 @@
       <c r="L164" s="2"/>
       <c r="M164" s="12"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>11</v>
       </c>
@@ -4217,7 +4291,7 @@
       <c r="L165" s="2"/>
       <c r="M165" s="12"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>12</v>
       </c>
@@ -4228,7 +4302,7 @@
       <c r="L166" s="2"/>
       <c r="M166" s="12"/>
     </row>
-    <row r="167" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>13</v>
       </c>
@@ -4245,7 +4319,7 @@
       <c r="L167" s="3"/>
       <c r="M167" s="12"/>
     </row>
-    <row r="168" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>15</v>
       </c>
@@ -4282,10 +4356,10 @@
       <c r="L168" s="3"/>
       <c r="M168" s="12"/>
     </row>
-    <row r="169" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
@@ -4300,7 +4374,7 @@
       <c r="L170" s="1"/>
       <c r="M170" s="12"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>9</v>
       </c>
@@ -4311,7 +4385,7 @@
       <c r="L171" s="2"/>
       <c r="M171" s="12"/>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>10</v>
       </c>
@@ -4322,7 +4396,7 @@
       <c r="L172" s="2"/>
       <c r="M172" s="12"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>11</v>
       </c>
@@ -4333,7 +4407,7 @@
       <c r="L173" s="2"/>
       <c r="M173" s="12"/>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>12</v>
       </c>
@@ -4344,7 +4418,7 @@
       <c r="L174" s="2"/>
       <c r="M174" s="12"/>
     </row>
-    <row r="175" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>13</v>
       </c>
@@ -4361,7 +4435,7 @@
       <c r="L175" s="3"/>
       <c r="M175" s="12"/>
     </row>
-    <row r="176" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Revert "Uren Registratie 9-11-15"
This reverts commit f0806529737a19014ca8c1267106abce42ca6748.
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="74">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -246,9 +246,6 @@
   </si>
   <si>
     <t>Michiel Ziek : Fahrettin Te Laat : Sven Te Laat :</t>
-  </si>
-  <si>
-    <t>Michiel niet aanwezig : Fahrettin niet aanwezig :</t>
   </si>
 </sst>
 </file>
@@ -914,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,7 +977,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
@@ -988,7 +985,7 @@
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.75124378109452739</v>
+        <v>0.76649746192893398</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1028,7 +1025,7 @@
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.61691542288557211</v>
+        <v>0.62944162436548223</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1064,11 +1061,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.93034825870646765</v>
+        <v>0.92893401015228427</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1104,11 +1101,11 @@
       <c r="K5" s="12"/>
       <c r="L5" s="7">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.57711442786069655</v>
+        <v>0.56852791878172593</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1142,11 +1139,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.95522388059701491</v>
+        <v>0.95431472081218272</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1182,11 +1179,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.92039800995024879</v>
+        <v>0.91878172588832485</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -3172,30 +3169,16 @@
         <v>9</v>
       </c>
       <c r="B91" s="12"/>
-      <c r="C91" s="10">
-        <v>0</v>
-      </c>
-      <c r="D91" s="10">
-        <v>0</v>
-      </c>
-      <c r="E91" s="9">
-        <v>4</v>
-      </c>
-      <c r="F91" s="9">
-        <v>4</v>
-      </c>
-      <c r="G91" s="9">
-        <v>4</v>
-      </c>
-      <c r="H91" s="9">
-        <v>4</v>
-      </c>
+      <c r="C91" s="19"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="56"/>
       <c r="I91" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="J91" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="J91" s="2"/>
       <c r="K91" s="12"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
@@ -3267,7 +3250,7 @@
         <v>15</v>
       </c>
       <c r="B96" s="11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C96" s="11">
         <f t="shared" ref="C96:H96" si="11">SUM(C91:C95)</f>
@@ -3279,19 +3262,19 @@
       </c>
       <c r="E96" s="11">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F96" s="11">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G96" s="11">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H96" s="11">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I96" s="11"/>
       <c r="J96" s="3"/>

</xml_diff>

<commit_message>
Update HUD en uren registratie 12-11-2015
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,15 +977,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.76415094339622647</v>
+        <v>0.76635514018691586</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1021,11 +1021,11 @@
       <c r="K3" s="12"/>
       <c r="L3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.58490566037735847</v>
+        <v>0.59345794392523366</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1061,11 +1061,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.93396226415094341</v>
+        <v>0.93457943925233644</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.58490566037735847</v>
+        <v>0.57943925233644855</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1139,11 +1139,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.95754716981132071</v>
+        <v>0.95794392523364491</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1179,11 +1179,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.92452830188679247</v>
+        <v>0.92523364485981308</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -3230,8 +3230,8 @@
       <c r="C93" s="41">
         <v>3</v>
       </c>
-      <c r="D93" s="10">
-        <v>0</v>
+      <c r="D93" s="46">
+        <v>1</v>
       </c>
       <c r="E93" s="9">
         <v>3</v>
@@ -3256,12 +3256,24 @@
         <v>12</v>
       </c>
       <c r="B94" s="12"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="56"/>
+      <c r="C94" s="41">
+        <v>2</v>
+      </c>
+      <c r="D94" s="9">
+        <v>2</v>
+      </c>
+      <c r="E94" s="9">
+        <v>2</v>
+      </c>
+      <c r="F94" s="10">
+        <v>0</v>
+      </c>
+      <c r="G94" s="9">
+        <v>2</v>
+      </c>
+      <c r="H94" s="42">
+        <v>2</v>
+      </c>
       <c r="I94" s="38"/>
       <c r="J94" s="2"/>
       <c r="K94" s="12"/>
@@ -3286,19 +3298,19 @@
         <v>15</v>
       </c>
       <c r="B96" s="11">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C96" s="11">
         <f t="shared" ref="C96:H96" si="11">SUM(C91:C95)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D96" s="11">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E96" s="11">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F96" s="11">
         <f t="shared" si="11"/>
@@ -3306,11 +3318,11 @@
       </c>
       <c r="G96" s="11">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H96" s="11">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I96" s="11"/>
       <c r="J96" s="3"/>

</xml_diff>

<commit_message>
Uren Registratie 12-11-2015 en kleine fix in scene 0
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L90" sqref="L90"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,11 +1139,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.95794392523364491</v>
+        <v>0.94859813084112155</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -3268,8 +3268,8 @@
       <c r="F94" s="10">
         <v>0</v>
       </c>
-      <c r="G94" s="9">
-        <v>2</v>
+      <c r="G94" s="10">
+        <v>0</v>
       </c>
       <c r="H94" s="42">
         <v>2</v>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="G96" s="11">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H96" s="11">
         <f t="shared" si="11"/>

</xml_diff>

<commit_message>
Uren Registratie update 20-11-15
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,11 +1139,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.93723849372384938</v>
+        <v>0.94560669456066948</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -3487,8 +3487,8 @@
       <c r="F103" s="22">
         <v>4</v>
       </c>
-      <c r="G103" s="23">
-        <v>0</v>
+      <c r="G103" s="24">
+        <v>2</v>
       </c>
       <c r="H103" s="50">
         <v>0</v>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="G104" s="11">
         <f t="shared" si="12"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H104" s="11">
         <f t="shared" si="12"/>

</xml_diff>

<commit_message>
Uren Registratie DE GOEDE 30-11-15
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\1. Game-Lab 1\8. GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L97" sqref="L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,15 +980,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.73897058823529416</v>
+        <v>0.71590909090909094</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.50735294117647056</v>
+        <v>0.52272727272727271</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.88970588235294112</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.56617647058823528</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.8970588235294118</v>
+        <v>0.9242424242424242</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.89338235294117652</v>
+        <v>0.92045454545454541</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -3748,8 +3748,8 @@
         <v>9</v>
       </c>
       <c r="B115" s="12"/>
-      <c r="C115" s="41">
-        <v>4</v>
+      <c r="C115" s="45">
+        <v>0</v>
       </c>
       <c r="D115" s="10">
         <v>0</v>
@@ -3777,9 +3777,7 @@
         <v>10</v>
       </c>
       <c r="B116" s="12"/>
-      <c r="C116" s="41">
-        <v>8</v>
-      </c>
+      <c r="C116" s="19"/>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
       <c r="F116" s="12"/>
@@ -3843,11 +3841,11 @@
         <v>15</v>
       </c>
       <c r="B120" s="11">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C120" s="11">
         <f t="shared" ref="C120:H120" si="14">SUM(C115:C119)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D120" s="11">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
Uren Registratie 01-12-2015 & small fixes
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\1. Game-Lab 1\8. GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L97" sqref="L97"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,15 +980,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.71590909090909094</v>
+        <v>0.72426470588235292</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1024,11 +1024,11 @@
       <c r="K3" s="12"/>
       <c r="L3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.52272727272727271</v>
+        <v>0.5220588235294118</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1064,11 +1064,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.91666666666666663</v>
+        <v>0.91911764705882348</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.58333333333333337</v>
+        <v>0.56617647058823528</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1142,11 +1142,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.9242424242424242</v>
+        <v>0.93382352941176472</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.92045454545454541</v>
+        <v>0.89338235294117652</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -3682,8 +3682,8 @@
       <c r="F111" s="23">
         <v>0</v>
       </c>
-      <c r="G111" s="23">
-        <v>0</v>
+      <c r="G111" s="24">
+        <v>3</v>
       </c>
       <c r="H111" s="44">
         <v>4</v>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="G112" s="11">
         <f t="shared" si="13"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H112" s="11">
         <f t="shared" si="13"/>
@@ -3777,12 +3777,24 @@
         <v>10</v>
       </c>
       <c r="B116" s="12"/>
-      <c r="C116" s="19"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-      <c r="G116" s="12"/>
-      <c r="H116" s="56"/>
+      <c r="C116" s="41">
+        <v>8</v>
+      </c>
+      <c r="D116" s="46">
+        <v>4</v>
+      </c>
+      <c r="E116" s="9">
+        <v>8</v>
+      </c>
+      <c r="F116" s="10">
+        <v>0</v>
+      </c>
+      <c r="G116" s="46">
+        <v>7</v>
+      </c>
+      <c r="H116" s="49">
+        <v>0</v>
+      </c>
       <c r="I116" s="36" t="s">
         <v>38</v>
       </c>
@@ -3841,19 +3853,19 @@
         <v>15</v>
       </c>
       <c r="B120" s="11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C120" s="11">
         <f t="shared" ref="C120:H120" si="14">SUM(C115:C119)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D120" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E120" s="11">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F120" s="11">
         <f t="shared" si="14"/>
@@ -3861,7 +3873,7 @@
       </c>
       <c r="G120" s="11">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H120" s="11">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
Uren Registratie, mijn reden van afwezigheid erbij gezet.
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\1. Game-Lab 1\8. GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="75">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Michiel Ziek : Fahrettin Te Laat : Sven Te Laat :</t>
+  </si>
+  <si>
+    <t>Rief geen laptop, werkt thuis</t>
   </si>
 </sst>
 </file>
@@ -915,7 +918,7 @@
   <dimension ref="A1:N176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L103" sqref="L103"/>
+      <selection activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,7 +3772,9 @@
       <c r="I115" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="J115" s="2"/>
+      <c r="J115" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K115" s="12"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -3798,7 +3803,9 @@
       <c r="I116" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="J116" s="2"/>
+      <c r="J116" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K116" s="12"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -3827,7 +3834,9 @@
       <c r="I117" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="J117" s="2"/>
+      <c r="J117" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K117" s="12"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uren Registratie 03-12-2015 & Bug Fixes
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\1. Game-Lab 1\8. GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="75">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K111" sqref="K111"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,11 +987,11 @@
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.72727272727272729</v>
+        <v>0.7345454545454545</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1067,11 +1067,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.92</v>
+        <v>0.92727272727272725</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1145,11 +1145,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.93090909090909091</v>
+        <v>0.93818181818181823</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1185,11 +1185,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.89454545454545453</v>
+        <v>0.90181818181818185</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -3844,14 +3844,28 @@
         <v>12</v>
       </c>
       <c r="B118" s="12"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="12"/>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
-      <c r="G118" s="12"/>
-      <c r="H118" s="56"/>
+      <c r="C118" s="41">
+        <v>2</v>
+      </c>
+      <c r="D118" s="10">
+        <v>0</v>
+      </c>
+      <c r="E118" s="9">
+        <v>2</v>
+      </c>
+      <c r="F118" s="10">
+        <v>0</v>
+      </c>
+      <c r="G118" s="9">
+        <v>2</v>
+      </c>
+      <c r="H118" s="42">
+        <v>2</v>
+      </c>
       <c r="I118" s="38"/>
-      <c r="J118" s="2"/>
+      <c r="J118" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="K118" s="12"/>
     </row>
     <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3878,7 +3892,7 @@
       </c>
       <c r="C120" s="11">
         <f t="shared" ref="C120:H120" si="14">SUM(C115:C119)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D120" s="11">
         <f t="shared" si="14"/>
@@ -3886,7 +3900,7 @@
       </c>
       <c r="E120" s="11">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F120" s="11">
         <f t="shared" si="14"/>
@@ -3894,11 +3908,11 @@
       </c>
       <c r="G120" s="11">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H120" s="11">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I120" s="11"/>
       <c r="J120" s="3"/>

</xml_diff>

<commit_message>
Uren Registratie 04-12-2015 & Bug Fix met raycastblock
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="75">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K115" sqref="K115"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,15 +983,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.7345454545454545</v>
+        <v>0.73309608540925264</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.51636363636363636</v>
+        <v>0.50533807829181498</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.92727272727272725</v>
+        <v>0.90747330960854089</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.56000000000000005</v>
+        <v>0.54804270462633453</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.93818181818181823</v>
+        <v>0.91814946619217086</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1185,11 +1185,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.90181818181818185</v>
+        <v>0.89679715302491103</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -3873,14 +3873,28 @@
         <v>13</v>
       </c>
       <c r="B119" s="11"/>
-      <c r="C119" s="20"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="57"/>
+      <c r="C119" s="43">
+        <v>4</v>
+      </c>
+      <c r="D119" s="23">
+        <v>0</v>
+      </c>
+      <c r="E119" s="23">
+        <v>0</v>
+      </c>
+      <c r="F119" s="23">
+        <v>0</v>
+      </c>
+      <c r="G119" s="23">
+        <v>0</v>
+      </c>
+      <c r="H119" s="44">
+        <v>4</v>
+      </c>
       <c r="I119" s="39"/>
-      <c r="J119" s="3"/>
+      <c r="J119" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="K119" s="12"/>
     </row>
     <row r="120" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3888,14 +3902,13 @@
         <v>15</v>
       </c>
       <c r="B120" s="11">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C120" s="11">
-        <f t="shared" ref="C120:H120" si="14">SUM(C115:C119)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D120" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="D120:H120" si="14">SUM(D115:D119)</f>
         <v>4</v>
       </c>
       <c r="E120" s="11">
@@ -3912,7 +3925,7 @@
       </c>
       <c r="H120" s="11">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I120" s="11"/>
       <c r="J120" s="3"/>

</xml_diff>

<commit_message>
Uren Registratie bijgewerkt roos en sven en minior bugg fixes
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="76">
   <si>
     <t>Fahrettin</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Rief geen laptop, werkt thuis</t>
+  </si>
+  <si>
+    <t>Totaal % Groep</t>
   </si>
 </sst>
 </file>
@@ -917,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K117" sqref="K117"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,11 +1070,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.90747330960854089</v>
+        <v>0.91459074733096091</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1145,11 +1148,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.91814946619217086</v>
+        <v>0.92526690391459077</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1232,6 +1235,13 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J9" s="27"/>
+      <c r="L9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="21">
+        <f>SUM(M2:M8)</f>
+        <v>4.5231316725978656</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3879,14 +3889,14 @@
       <c r="D119" s="23">
         <v>0</v>
       </c>
-      <c r="E119" s="23">
-        <v>0</v>
+      <c r="E119" s="24">
+        <v>2</v>
       </c>
       <c r="F119" s="23">
         <v>0</v>
       </c>
-      <c r="G119" s="23">
-        <v>0</v>
+      <c r="G119" s="24">
+        <v>2</v>
       </c>
       <c r="H119" s="44">
         <v>4</v>
@@ -3913,7 +3923,7 @@
       </c>
       <c r="E120" s="11">
         <f t="shared" si="14"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F120" s="11">
         <f t="shared" si="14"/>
@@ -3921,7 +3931,7 @@
       </c>
       <c r="G120" s="11">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H120" s="11">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
Uren Registratie nu goed
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -920,23 +920,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="8" width="10.88671875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.109375" customWidth="1"/>
-    <col min="11" max="12" width="22.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="8" width="10.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.140625" customWidth="1"/>
+    <col min="11" max="12" width="22.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
@@ -971,7 +971,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -986,7 +986,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
@@ -994,13 +994,13 @@
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.69830508474576269</v>
+        <v>0.69594594594594594</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1034,13 +1034,13 @@
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.48135593220338985</v>
+        <v>0.47972972972972971</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1070,17 +1070,17 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.91864406779661012</v>
+        <v>0.91891891891891897</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1110,17 +1110,17 @@
       <c r="K5" s="12"/>
       <c r="L5" s="7">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.56271186440677967</v>
+        <v>0.56418918918918914</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1148,17 +1148,17 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.92203389830508475</v>
+        <v>0.92905405405405406</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1188,17 +1188,17 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.89491525423728813</v>
+        <v>0.90202702702702697</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1233,17 +1233,17 @@
       <c r="J8" s="26"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J9" s="27"/>
       <c r="L9" s="7" t="s">
         <v>75</v>
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.477966101694915</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.4898648648648649</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1318,7 +1318,7 @@
       <c r="J12" s="29"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -1440,10 +1440,10 @@
       <c r="J16" s="26"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="J18" s="28"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1487,7 @@
       <c r="J19" s="29"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="J22" s="29"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
@@ -1640,8 +1640,8 @@
       <c r="J24" s="3"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
@@ -1840,8 +1840,8 @@
       <c r="J32" s="3"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>9</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>13</v>
       </c>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>15</v>
       </c>
@@ -2042,8 +2042,8 @@
       <c r="J40" s="3"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="12"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>10</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="K44" s="12"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>13</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>15</v>
       </c>
@@ -2242,8 +2242,8 @@
       <c r="J48" s="3"/>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>9</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>10</v>
       </c>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="K52" s="12"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>11</v>
       </c>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>15</v>
       </c>
@@ -2440,8 +2440,8 @@
       <c r="J56" s="3"/>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>24</v>
       </c>
@@ -2456,7 +2456,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>9</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="K59" s="12"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>10</v>
       </c>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>11</v>
       </c>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="K61" s="12"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>12</v>
       </c>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="K62" s="12"/>
     </row>
-    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>13</v>
       </c>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>15</v>
       </c>
@@ -2642,7 +2642,7 @@
       <c r="J64" s="3"/>
       <c r="K64" s="12"/>
     </row>
-    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="18"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -2653,7 +2653,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2668,7 +2668,7 @@
       <c r="J66" s="31"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2683,7 +2683,7 @@
       <c r="J67" s="33"/>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="J68" s="33"/>
       <c r="K68" s="12"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2713,7 +2713,7 @@
       <c r="J69" s="33"/>
       <c r="K69" s="12"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -2728,7 +2728,7 @@
       <c r="J70" s="33"/>
       <c r="K70" s="12"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2743,7 +2743,7 @@
       <c r="J71" s="35"/>
       <c r="K71" s="12"/>
     </row>
-    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>15</v>
       </c>
@@ -2778,8 +2778,8 @@
       <c r="J72" s="3"/>
       <c r="K72" s="12"/>
     </row>
-    <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2794,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="12"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>9</v>
       </c>
@@ -2811,7 +2811,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>10</v>
       </c>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="K76" s="12"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>11</v>
       </c>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="K77" s="12"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>12</v>
       </c>
@@ -2900,7 +2900,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="12"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>13</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="J79" s="3"/>
       <c r="K79" s="12"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>15</v>
       </c>
@@ -2962,8 +2962,8 @@
       <c r="J80" s="3"/>
       <c r="K80" s="12"/>
     </row>
-    <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>27</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="12"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>9</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="K83" s="12"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>10</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="K84" s="12"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>11</v>
       </c>
@@ -3071,7 +3071,7 @@
       </c>
       <c r="K85" s="12"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>12</v>
       </c>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="K86" s="12"/>
     </row>
-    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>13</v>
       </c>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="K87" s="12"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>15</v>
       </c>
@@ -3164,8 +3164,8 @@
       <c r="J88" s="3"/>
       <c r="K88" s="12"/>
     </row>
-    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>28</v>
       </c>
@@ -3180,7 +3180,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>9</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>10</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="12"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>11</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="12"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>12</v>
       </c>
@@ -3294,7 +3294,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="12"/>
     </row>
-    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>13</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="J95" s="3"/>
       <c r="K95" s="12"/>
     </row>
-    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>15</v>
       </c>
@@ -3356,8 +3356,8 @@
       <c r="J96" s="3"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>29</v>
       </c>
@@ -3372,7 +3372,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="12"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>9</v>
       </c>
@@ -3401,7 +3401,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="12"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>10</v>
       </c>
@@ -3430,7 +3430,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="12"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>11</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="12"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>12</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="12"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>13</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="12"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>15</v>
       </c>
@@ -3548,8 +3548,8 @@
       <c r="J104" s="3"/>
       <c r="K104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>30</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="12"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>9</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>10</v>
       </c>
@@ -3622,7 +3622,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="12"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>11</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="12"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>12</v>
       </c>
@@ -3678,7 +3678,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="12"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>13</v>
       </c>
@@ -3705,7 +3705,7 @@
       <c r="J111" s="3"/>
       <c r="K111" s="12"/>
     </row>
-    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>15</v>
       </c>
@@ -3740,8 +3740,8 @@
       <c r="J112" s="3"/>
       <c r="K112" s="12"/>
     </row>
-    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>31</v>
       </c>
@@ -3756,7 +3756,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="12"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>9</v>
       </c>
@@ -3787,7 +3787,7 @@
       </c>
       <c r="K115" s="12"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>10</v>
       </c>
@@ -3818,7 +3818,7 @@
       </c>
       <c r="K116" s="12"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>11</v>
       </c>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="K117" s="12"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>12</v>
       </c>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="K118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>13</v>
       </c>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="K119" s="12"/>
     </row>
-    <row r="120" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>15</v>
       </c>
@@ -3941,8 +3941,8 @@
       <c r="J120" s="3"/>
       <c r="K120" s="12"/>
     </row>
-    <row r="121" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>32</v>
       </c>
@@ -3957,7 +3957,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="12"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>9</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="12"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>10</v>
       </c>
@@ -4015,7 +4015,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="12"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>11</v>
       </c>
@@ -4027,16 +4027,16 @@
         <v>0</v>
       </c>
       <c r="E125" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F125" s="9">
-        <v>2</v>
-      </c>
-      <c r="G125" s="10">
-        <v>0</v>
-      </c>
-      <c r="H125" s="49">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G125" s="9">
+        <v>3</v>
+      </c>
+      <c r="H125" s="42">
+        <v>3</v>
       </c>
       <c r="I125" s="37" t="s">
         <v>7</v>
@@ -4044,7 +4044,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="12"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>12</v>
       </c>
@@ -4059,7 +4059,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="12"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>13</v>
       </c>
@@ -4074,12 +4074,12 @@
       <c r="J127" s="3"/>
       <c r="K127" s="12"/>
     </row>
-    <row r="128" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B128" s="11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C128" s="11">
         <f t="shared" ref="C128:H128" si="15">SUM(C123:C127)</f>
@@ -4091,26 +4091,26 @@
       </c>
       <c r="E128" s="11">
         <f t="shared" si="15"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F128" s="11">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G128" s="11">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H128" s="11">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I128" s="11"/>
       <c r="J128" s="3"/>
       <c r="K128" s="12"/>
     </row>
-    <row r="129" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>33</v>
       </c>
@@ -4125,7 +4125,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="12"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>9</v>
       </c>
@@ -4142,7 +4142,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="12"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>10</v>
       </c>
@@ -4159,7 +4159,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="12"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>11</v>
       </c>
@@ -4176,7 +4176,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="12"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>12</v>
       </c>
@@ -4191,7 +4191,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="12"/>
     </row>
-    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>13</v>
       </c>
@@ -4206,7 +4206,7 @@
       <c r="J135" s="3"/>
       <c r="K135" s="12"/>
     </row>
-    <row r="136" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>15</v>
       </c>
@@ -4241,8 +4241,8 @@
       <c r="J136" s="3"/>
       <c r="K136" s="12"/>
     </row>
-    <row r="137" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -4257,7 +4257,7 @@
       <c r="J138" s="31"/>
       <c r="K138" s="12"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -4272,7 +4272,7 @@
       <c r="J139" s="33"/>
       <c r="K139" s="12"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -4287,7 +4287,7 @@
       <c r="J140" s="33"/>
       <c r="K140" s="12"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -4302,7 +4302,7 @@
       <c r="J141" s="33"/>
       <c r="K141" s="12"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>12</v>
       </c>
@@ -4317,7 +4317,7 @@
       <c r="J142" s="33"/>
       <c r="K142" s="12"/>
     </row>
-    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -4332,7 +4332,7 @@
       <c r="J143" s="35"/>
       <c r="K143" s="12"/>
     </row>
-    <row r="144" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>15</v>
       </c>
@@ -4367,8 +4367,8 @@
       <c r="J144" s="3"/>
       <c r="K144" s="12"/>
     </row>
-    <row r="145" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>46</v>
       </c>
@@ -4383,7 +4383,7 @@
       <c r="J146" s="31"/>
       <c r="K146" s="12"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -4398,7 +4398,7 @@
       <c r="J147" s="33"/>
       <c r="K147" s="12"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -4413,7 +4413,7 @@
       <c r="J148" s="33"/>
       <c r="K148" s="12"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -4428,7 +4428,7 @@
       <c r="J149" s="33"/>
       <c r="K149" s="12"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>12</v>
       </c>
@@ -4443,7 +4443,7 @@
       <c r="J150" s="33"/>
       <c r="K150" s="12"/>
     </row>
-    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>13</v>
       </c>
@@ -4458,7 +4458,7 @@
       <c r="J151" s="35"/>
       <c r="K151" s="12"/>
     </row>
-    <row r="152" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>15</v>
       </c>
@@ -4493,8 +4493,8 @@
       <c r="J152" s="3"/>
       <c r="K152" s="12"/>
     </row>
-    <row r="153" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>35</v>
       </c>
@@ -4509,7 +4509,7 @@
       <c r="J154" s="1"/>
       <c r="K154" s="12"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>9</v>
       </c>
@@ -4526,7 +4526,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="12"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>10</v>
       </c>
@@ -4543,7 +4543,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="12"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>11</v>
       </c>
@@ -4560,7 +4560,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="12"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>12</v>
       </c>
@@ -4575,7 +4575,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="12"/>
     </row>
-    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>13</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="J159" s="3"/>
       <c r="K159" s="12"/>
     </row>
-    <row r="160" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>15</v>
       </c>
@@ -4625,8 +4625,8 @@
       <c r="J160" s="3"/>
       <c r="K160" s="12"/>
     </row>
-    <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>36</v>
       </c>
@@ -4641,7 +4641,7 @@
       <c r="J162" s="1"/>
       <c r="K162" s="12"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>9</v>
       </c>
@@ -4658,7 +4658,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="12"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>10</v>
       </c>
@@ -4675,7 +4675,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="12"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>11</v>
       </c>
@@ -4692,7 +4692,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="12"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>12</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="12"/>
     </row>
-    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>13</v>
       </c>
@@ -4722,7 +4722,7 @@
       <c r="J167" s="3"/>
       <c r="K167" s="12"/>
     </row>
-    <row r="168" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>15</v>
       </c>
@@ -4757,8 +4757,8 @@
       <c r="J168" s="3"/>
       <c r="K168" s="12"/>
     </row>
-    <row r="169" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>37</v>
       </c>
@@ -4773,7 +4773,7 @@
       <c r="J170" s="1"/>
       <c r="K170" s="12"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>9</v>
       </c>
@@ -4790,7 +4790,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="12"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>10</v>
       </c>
@@ -4807,7 +4807,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="12"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>11</v>
       </c>
@@ -4824,7 +4824,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="12"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>12</v>
       </c>
@@ -4839,7 +4839,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="12"/>
     </row>
-    <row r="175" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>13</v>
       </c>
@@ -4854,7 +4854,7 @@
       <c r="J175" s="3"/>
       <c r="K175" s="12"/>
     </row>
-    <row r="176" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
change urenregistratie vorige week woensdag
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,7 +986,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
@@ -994,7 +994,7 @@
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.68627450980392157</v>
+        <v>0.68852459016393441</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.47058823529411764</v>
+        <v>0.47213114754098362</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1070,11 +1070,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.90849673202614378</v>
+        <v>0.90819672131147544</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1110,11 +1110,11 @@
       <c r="K5" s="12"/>
       <c r="L5" s="7">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.565359477124183</v>
+        <v>0.56393442622950818</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1148,11 +1148,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.90849673202614378</v>
+        <v>0.90819672131147544</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1188,11 +1188,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.89215686274509809</v>
+        <v>0.8918032786885246</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.4313725490196072</v>
+        <v>4.4327868852459016</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4027,16 +4027,16 @@
         <v>0</v>
       </c>
       <c r="E125" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F125" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G125" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H125" s="42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I125" s="37" t="s">
         <v>7</v>
@@ -4103,7 +4103,7 @@
         <v>15</v>
       </c>
       <c r="B128" s="11">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C128" s="11">
         <f t="shared" ref="C128:H128" si="15">SUM(C123:C127)</f>
@@ -4115,19 +4115,19 @@
       </c>
       <c r="E128" s="11">
         <f t="shared" si="15"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F128" s="11">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G128" s="11">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H128" s="11">
         <f t="shared" si="15"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I128" s="11"/>
       <c r="J128" s="3"/>

</xml_diff>

<commit_message>
Uren Registratie 05-01-2016 & 06-01-2016
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2e Schooljaar\1. Game-Lab 1\8. GitHub\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -920,23 +920,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G156" sqref="G156"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="8" width="10.88671875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.109375" customWidth="1"/>
-    <col min="11" max="12" width="22.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="8" width="10.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.140625" customWidth="1"/>
+    <col min="11" max="12" width="22.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
@@ -971,7 +971,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -986,21 +986,21 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.65846153846153843</v>
+        <v>0.6811594202898551</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1030,17 +1030,17 @@
       <c r="K3" s="12"/>
       <c r="L3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.45846153846153848</v>
+        <v>0.45797101449275363</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1070,38 +1070,38 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.91384615384615386</v>
+        <v>0.91884057971014488</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>7</v>
@@ -1110,17 +1110,17 @@
       <c r="K5" s="12"/>
       <c r="L5" s="7">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.57846153846153847</v>
+        <v>0.58550724637681162</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1148,17 +1148,17 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.90153846153846151</v>
+        <v>0.90724637681159426</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1188,62 +1188,62 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.89846153846153842</v>
+        <v>0.90434782608695652</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="11">
         <f t="shared" ref="C8:H8" si="0">SUM(C3:C7)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="26"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J9" s="27"/>
       <c r="L9" s="7" t="s">
         <v>75</v>
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.4092307692307688</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.4550724637681158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1318,28 +1318,28 @@
       <c r="J12" s="29"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="41">
+        <v>6</v>
+      </c>
+      <c r="D13" s="46">
         <v>5</v>
       </c>
-      <c r="D13" s="46">
-        <v>4</v>
-      </c>
       <c r="E13" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G13" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I13" s="37" t="s">
         <v>7</v>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1405,45 +1405,45 @@
       </c>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="11">
         <f t="shared" ref="C16:H16" si="1">SUM(C11:C15)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="26"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="J18" s="28"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1487,7 @@
       <c r="J19" s="29"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1518,28 +1518,28 @@
       </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="41">
+        <v>6</v>
+      </c>
+      <c r="D21" s="9">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9">
+        <v>6</v>
+      </c>
+      <c r="F21" s="46">
         <v>5</v>
       </c>
-      <c r="D21" s="9">
-        <v>5</v>
-      </c>
-      <c r="E21" s="9">
-        <v>5</v>
-      </c>
-      <c r="F21" s="46">
-        <v>4</v>
-      </c>
       <c r="G21" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I21" s="37" t="s">
         <v>7</v>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="J22" s="29"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
@@ -1605,43 +1605,43 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="11">
         <f t="shared" ref="C24:H24" si="2">SUM(C19:C23)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D24" s="11">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G24" s="11">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H24" s="11">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I24" s="11"/>
       <c r="J24" s="3"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1685,13 +1685,13 @@
       <c r="J27" s="2"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28" s="46">
         <v>3</v>
@@ -1716,25 +1716,25 @@
       </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F29" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G29" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H29" s="49">
         <v>0</v>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I30" s="38"/>
       <c r="J30" s="2" t="s">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
@@ -1805,43 +1805,43 @@
       </c>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" s="11">
         <f t="shared" ref="C32:H32" si="3">SUM(C27:C31)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" s="11">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G32" s="11">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H32" s="11">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="3"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>9</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>4</v>
       </c>
       <c r="F35" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G35" s="9">
         <v>4</v>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -1918,28 +1918,28 @@
       </c>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D37" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E37" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F37" s="10">
         <v>0</v>
       </c>
       <c r="G37" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H37" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I37" s="37" t="s">
         <v>7</v>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>13</v>
       </c>
@@ -2007,43 +2007,43 @@
       </c>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B40" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C40" s="11">
         <f t="shared" ref="C40:H40" si="4">SUM(C35:C39)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D40" s="11">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E40" s="11">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F40" s="11">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G40" s="11">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H40" s="11">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I40" s="11"/>
       <c r="J40" s="3"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="12"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>10</v>
       </c>
@@ -2120,28 +2120,28 @@
       </c>
       <c r="K44" s="12"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D45" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E45" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F45" s="10">
         <v>0</v>
       </c>
       <c r="G45" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H45" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I45" s="37" t="s">
         <v>7</v>
@@ -2149,7 +2149,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G46" s="9">
         <v>2</v>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>13</v>
       </c>
@@ -2207,43 +2207,43 @@
       </c>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C48" s="11">
         <f t="shared" ref="C48:H48" si="5">SUM(C43:C47)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D48" s="11">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E48" s="11">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F48" s="11">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G48" s="11">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H48" s="11">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I48" s="11"/>
       <c r="J48" s="3"/>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>9</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>10</v>
       </c>
@@ -2320,28 +2320,28 @@
       </c>
       <c r="K52" s="12"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D53" s="10">
         <v>0</v>
       </c>
       <c r="E53" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F53" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G53" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H53" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I53" s="37" t="s">
         <v>7</v>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E55" s="22">
         <v>4</v>
@@ -2405,43 +2405,43 @@
       <c r="J55" s="3"/>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B56" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C56" s="11">
         <f t="shared" ref="C56:H56" si="6">SUM(C51:C55)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56" s="11">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F56" s="11">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G56" s="11">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H56" s="11">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I56" s="11"/>
       <c r="J56" s="3"/>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>24</v>
       </c>
@@ -2456,7 +2456,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>9</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="K59" s="12"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>10</v>
       </c>
@@ -2518,28 +2518,28 @@
       </c>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D61" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E61" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F61" s="10">
         <v>0</v>
       </c>
       <c r="G61" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H61" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I61" s="37" t="s">
         <v>7</v>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="K61" s="12"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>12</v>
       </c>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="K62" s="12"/>
     </row>
-    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>13</v>
       </c>
@@ -2592,8 +2592,8 @@
       <c r="E63" s="22">
         <v>4</v>
       </c>
-      <c r="F63" s="23">
-        <v>0</v>
+      <c r="F63" s="24">
+        <v>1</v>
       </c>
       <c r="G63" s="22">
         <v>4</v>
@@ -2607,42 +2607,42 @@
       </c>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B64" s="11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C64" s="11">
         <f t="shared" ref="C64:H64" si="7">SUM(C59:C63)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D64" s="11">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E64" s="11">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F64" s="11">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="11">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H64" s="11">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I64" s="11"/>
       <c r="J64" s="3"/>
       <c r="K64" s="12"/>
     </row>
-    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="18"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -2653,7 +2653,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2668,7 +2668,7 @@
       <c r="J66" s="31"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2683,7 +2683,7 @@
       <c r="J67" s="33"/>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2698,7 +2698,7 @@
       <c r="J68" s="33"/>
       <c r="K68" s="12"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2713,7 +2713,7 @@
       <c r="J69" s="33"/>
       <c r="K69" s="12"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -2728,7 +2728,7 @@
       <c r="J70" s="33"/>
       <c r="K70" s="12"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2743,7 +2743,7 @@
       <c r="J71" s="35"/>
       <c r="K71" s="12"/>
     </row>
-    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>15</v>
       </c>
@@ -2778,8 +2778,8 @@
       <c r="J72" s="3"/>
       <c r="K72" s="12"/>
     </row>
-    <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2794,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="12"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>9</v>
       </c>
@@ -2811,7 +2811,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>10</v>
       </c>
@@ -2842,28 +2842,28 @@
       </c>
       <c r="K76" s="12"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B77" s="12"/>
       <c r="C77" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D77" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E77" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F77" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G77" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H77" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I77" s="37" t="s">
         <v>7</v>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="K77" s="12"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>12</v>
       </c>
@@ -2900,7 +2900,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="12"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>13</v>
       </c>
@@ -2927,43 +2927,43 @@
       <c r="J79" s="3"/>
       <c r="K79" s="12"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B80" s="11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C80" s="11">
         <f t="shared" ref="C80:H80" si="9">SUM(C75:C79)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D80" s="11">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E80" s="11">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F80" s="11">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G80" s="11">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H80" s="11">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I80" s="11"/>
       <c r="J80" s="3"/>
       <c r="K80" s="12"/>
     </row>
-    <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>27</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="12"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>9</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="K83" s="12"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>10</v>
       </c>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="K84" s="12"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>11</v>
       </c>
@@ -3071,7 +3071,7 @@
       </c>
       <c r="K85" s="12"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>12</v>
       </c>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="K86" s="12"/>
     </row>
-    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>13</v>
       </c>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="K87" s="12"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>15</v>
       </c>
@@ -3164,8 +3164,8 @@
       <c r="J88" s="3"/>
       <c r="K88" s="12"/>
     </row>
-    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>28</v>
       </c>
@@ -3180,7 +3180,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>9</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>10</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="12"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>11</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="12"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>12</v>
       </c>
@@ -3294,7 +3294,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="12"/>
     </row>
-    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>13</v>
       </c>
@@ -3321,7 +3321,7 @@
       <c r="J95" s="3"/>
       <c r="K95" s="12"/>
     </row>
-    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>15</v>
       </c>
@@ -3356,8 +3356,8 @@
       <c r="J96" s="3"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>29</v>
       </c>
@@ -3372,7 +3372,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="12"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>9</v>
       </c>
@@ -3401,7 +3401,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="12"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>10</v>
       </c>
@@ -3430,7 +3430,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="12"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>11</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="12"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>12</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="12"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>13</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="12"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>15</v>
       </c>
@@ -3548,8 +3548,8 @@
       <c r="J104" s="3"/>
       <c r="K104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>30</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="12"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>9</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>10</v>
       </c>
@@ -3622,7 +3622,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="12"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>11</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="12"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>12</v>
       </c>
@@ -3678,7 +3678,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="12"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>13</v>
       </c>
@@ -3705,7 +3705,7 @@
       <c r="J111" s="3"/>
       <c r="K111" s="12"/>
     </row>
-    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>15</v>
       </c>
@@ -3740,8 +3740,8 @@
       <c r="J112" s="3"/>
       <c r="K112" s="12"/>
     </row>
-    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>31</v>
       </c>
@@ -3756,7 +3756,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="12"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>9</v>
       </c>
@@ -3787,7 +3787,7 @@
       </c>
       <c r="K115" s="12"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>10</v>
       </c>
@@ -3818,7 +3818,7 @@
       </c>
       <c r="K116" s="12"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>11</v>
       </c>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="K117" s="12"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>12</v>
       </c>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="K118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>13</v>
       </c>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="K119" s="12"/>
     </row>
-    <row r="120" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>15</v>
       </c>
@@ -3941,8 +3941,8 @@
       <c r="J120" s="3"/>
       <c r="K120" s="12"/>
     </row>
-    <row r="121" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>32</v>
       </c>
@@ -3957,7 +3957,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="12"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>9</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="12"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>10</v>
       </c>
@@ -4015,7 +4015,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="12"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>11</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="12"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>12</v>
       </c>
@@ -4071,7 +4071,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="12"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>13</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="J127" s="3"/>
       <c r="K127" s="12"/>
     </row>
-    <row r="128" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>15</v>
       </c>
@@ -4133,8 +4133,8 @@
       <c r="J128" s="3"/>
       <c r="K128" s="12"/>
     </row>
-    <row r="129" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>33</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="12"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>9</v>
       </c>
@@ -4178,7 +4178,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="12"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>10</v>
       </c>
@@ -4207,7 +4207,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="12"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>11</v>
       </c>
@@ -4236,7 +4236,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="12"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>12</v>
       </c>
@@ -4263,7 +4263,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="12"/>
     </row>
-    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>13</v>
       </c>
@@ -4290,7 +4290,7 @@
       <c r="J135" s="3"/>
       <c r="K135" s="12"/>
     </row>
-    <row r="136" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>15</v>
       </c>
@@ -4325,8 +4325,8 @@
       <c r="J136" s="3"/>
       <c r="K136" s="12"/>
     </row>
-    <row r="137" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -4341,7 +4341,7 @@
       <c r="J138" s="31"/>
       <c r="K138" s="12"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -4356,7 +4356,7 @@
       <c r="J139" s="33"/>
       <c r="K139" s="12"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -4371,7 +4371,7 @@
       <c r="J140" s="33"/>
       <c r="K140" s="12"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -4386,7 +4386,7 @@
       <c r="J141" s="33"/>
       <c r="K141" s="12"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>12</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="J142" s="33"/>
       <c r="K142" s="12"/>
     </row>
-    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -4416,7 +4416,7 @@
       <c r="J143" s="35"/>
       <c r="K143" s="12"/>
     </row>
-    <row r="144" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>15</v>
       </c>
@@ -4451,8 +4451,8 @@
       <c r="J144" s="3"/>
       <c r="K144" s="12"/>
     </row>
-    <row r="145" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>46</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="J146" s="31"/>
       <c r="K146" s="12"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -4482,7 +4482,7 @@
       <c r="J147" s="33"/>
       <c r="K147" s="12"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -4497,7 +4497,7 @@
       <c r="J148" s="33"/>
       <c r="K148" s="12"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -4512,7 +4512,7 @@
       <c r="J149" s="33"/>
       <c r="K149" s="12"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>12</v>
       </c>
@@ -4527,7 +4527,7 @@
       <c r="J150" s="33"/>
       <c r="K150" s="12"/>
     </row>
-    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>13</v>
       </c>
@@ -4542,7 +4542,7 @@
       <c r="J151" s="35"/>
       <c r="K151" s="12"/>
     </row>
-    <row r="152" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>15</v>
       </c>
@@ -4577,8 +4577,8 @@
       <c r="J152" s="3"/>
       <c r="K152" s="12"/>
     </row>
-    <row r="153" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>35</v>
       </c>
@@ -4593,7 +4593,7 @@
       <c r="J154" s="1"/>
       <c r="K154" s="12"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>9</v>
       </c>
@@ -4622,41 +4622,65 @@
       <c r="J155" s="2"/>
       <c r="K155" s="12"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B156" s="12"/>
-      <c r="C156" s="19"/>
-      <c r="D156" s="12"/>
-      <c r="E156" s="12"/>
-      <c r="F156" s="12"/>
-      <c r="G156" s="12"/>
-      <c r="H156" s="56"/>
+      <c r="C156" s="41">
+        <v>6</v>
+      </c>
+      <c r="D156" s="10">
+        <v>0</v>
+      </c>
+      <c r="E156" s="9">
+        <v>6</v>
+      </c>
+      <c r="F156" s="10">
+        <v>0</v>
+      </c>
+      <c r="G156" s="9">
+        <v>6</v>
+      </c>
+      <c r="H156" s="42">
+        <v>6</v>
+      </c>
       <c r="I156" s="36" t="s">
         <v>38</v>
       </c>
       <c r="J156" s="2"/>
       <c r="K156" s="12"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B157" s="12"/>
-      <c r="C157" s="19"/>
-      <c r="D157" s="12"/>
-      <c r="E157" s="12"/>
-      <c r="F157" s="12"/>
-      <c r="G157" s="12"/>
-      <c r="H157" s="56"/>
+      <c r="C157" s="41">
+        <v>5</v>
+      </c>
+      <c r="D157" s="10">
+        <v>0</v>
+      </c>
+      <c r="E157" s="9">
+        <v>5</v>
+      </c>
+      <c r="F157" s="9">
+        <v>5</v>
+      </c>
+      <c r="G157" s="9">
+        <v>5</v>
+      </c>
+      <c r="H157" s="42">
+        <v>5</v>
+      </c>
       <c r="I157" s="37" t="s">
         <v>7</v>
       </c>
       <c r="J157" s="2"/>
       <c r="K157" s="12"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>12</v>
       </c>
@@ -4671,7 +4695,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="12"/>
     </row>
-    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>13</v>
       </c>
@@ -4686,16 +4710,16 @@
       <c r="J159" s="3"/>
       <c r="K159" s="12"/>
     </row>
-    <row r="160" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B160" s="11">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C160" s="11">
         <f t="shared" ref="C160:H160" si="19">SUM(C155:C159)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D160" s="11">
         <f t="shared" si="19"/>
@@ -4703,26 +4727,26 @@
       </c>
       <c r="E160" s="11">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F160" s="11">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G160" s="11">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H160" s="11">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I160" s="11"/>
       <c r="J160" s="3"/>
       <c r="K160" s="12"/>
     </row>
-    <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>36</v>
       </c>
@@ -4737,7 +4761,7 @@
       <c r="J162" s="1"/>
       <c r="K162" s="12"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>9</v>
       </c>
@@ -4754,7 +4778,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="12"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>10</v>
       </c>
@@ -4771,7 +4795,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="12"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>11</v>
       </c>
@@ -4788,7 +4812,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="12"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>12</v>
       </c>
@@ -4803,7 +4827,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="12"/>
     </row>
-    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>13</v>
       </c>
@@ -4818,7 +4842,7 @@
       <c r="J167" s="3"/>
       <c r="K167" s="12"/>
     </row>
-    <row r="168" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>15</v>
       </c>
@@ -4853,8 +4877,8 @@
       <c r="J168" s="3"/>
       <c r="K168" s="12"/>
     </row>
-    <row r="169" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>37</v>
       </c>
@@ -4869,7 +4893,7 @@
       <c r="J170" s="1"/>
       <c r="K170" s="12"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>9</v>
       </c>
@@ -4886,7 +4910,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="12"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>10</v>
       </c>
@@ -4903,7 +4927,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="12"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>11</v>
       </c>
@@ -4920,7 +4944,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="12"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>12</v>
       </c>
@@ -4935,7 +4959,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="12"/>
     </row>
-    <row r="175" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>13</v>
       </c>
@@ -4950,7 +4974,7 @@
       <c r="J175" s="3"/>
       <c r="K175" s="12"/>
     </row>
-    <row r="176" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Uren registratie van michiel aangepast omdat die wel aanwezig was later en small bug fix met emptyslots
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -921,7 +921,7 @@
   <dimension ref="A1:N176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,11 +1030,11 @@
       <c r="K3" s="12"/>
       <c r="L3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.45797101449275363</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.4550724637681158</v>
+        <v>4.4637681159420284</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4659,8 +4659,8 @@
       <c r="C157" s="41">
         <v>5</v>
       </c>
-      <c r="D157" s="10">
-        <v>0</v>
+      <c r="D157" s="46">
+        <v>3</v>
       </c>
       <c r="E157" s="9">
         <v>5</v>
@@ -4723,7 +4723,7 @@
       </c>
       <c r="D160" s="11">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E160" s="11">
         <f t="shared" si="19"/>

</xml_diff>

<commit_message>
Uren Registratie 07-01-2016 & Animatie van termiet gefixed
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -921,7 +921,7 @@
   <dimension ref="A1:N176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+      <selection activeCell="L163" sqref="L163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,11 +990,11 @@
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.6811594202898551</v>
+        <v>0.69275362318840583</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1070,11 +1070,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.91884057971014488</v>
+        <v>0.93043478260869561</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1110,11 +1110,11 @@
       <c r="K5" s="12"/>
       <c r="L5" s="7">
         <f>F8+F16+F24+F32+F40+F48+F56+F64+F72+F80+F88+F96+F104+F112+F120+F128+F136+F144+F152+F160+F168+F176</f>
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.58550724637681162</v>
+        <v>0.59710144927536235</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1148,11 +1148,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.90724637681159426</v>
+        <v>0.91884057971014488</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1188,11 +1188,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.90434782608695652</v>
+        <v>0.90144927536231889</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.4637681159420284</v>
+        <v>4.5072463768115947</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4671,8 +4671,8 @@
       <c r="G157" s="9">
         <v>5</v>
       </c>
-      <c r="H157" s="42">
-        <v>5</v>
+      <c r="H157" s="49">
+        <v>0</v>
       </c>
       <c r="I157" s="37" t="s">
         <v>7</v>
@@ -4685,12 +4685,24 @@
         <v>12</v>
       </c>
       <c r="B158" s="12"/>
-      <c r="C158" s="19"/>
-      <c r="D158" s="12"/>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12"/>
-      <c r="G158" s="12"/>
-      <c r="H158" s="56"/>
+      <c r="C158" s="41">
+        <v>4</v>
+      </c>
+      <c r="D158" s="10">
+        <v>0</v>
+      </c>
+      <c r="E158" s="9">
+        <v>4</v>
+      </c>
+      <c r="F158" s="9">
+        <v>4</v>
+      </c>
+      <c r="G158" s="9">
+        <v>4</v>
+      </c>
+      <c r="H158" s="42">
+        <v>4</v>
+      </c>
       <c r="I158" s="38"/>
       <c r="J158" s="2"/>
       <c r="K158" s="12"/>
@@ -4719,7 +4731,7 @@
       </c>
       <c r="C160" s="11">
         <f t="shared" ref="C160:H160" si="19">SUM(C155:C159)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D160" s="11">
         <f t="shared" si="19"/>
@@ -4727,19 +4739,19 @@
       </c>
       <c r="E160" s="11">
         <f t="shared" si="19"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F160" s="11">
         <f t="shared" si="19"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G160" s="11">
         <f t="shared" si="19"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H160" s="11">
         <f t="shared" si="19"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I160" s="11"/>
       <c r="J160" s="3"/>

</xml_diff>

<commit_message>
Uren Registratie 12-01-2015 & LoadingScreen Toegevoegd
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L164" sqref="L164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,15 +989,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176</f>
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176</f>
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.71148459383753504</v>
+        <v>0.71780821917808224</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
@@ -1033,11 +1033,11 @@
       <c r="K3" s="12"/>
       <c r="L3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176</f>
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.45098039215686275</v>
+        <v>0.45479452054794522</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
@@ -1073,11 +1073,11 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176</f>
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.91596638655462181</v>
+        <v>0.9178082191780822</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.58823529411764708</v>
+        <v>0.57534246575342463</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
@@ -1151,11 +1151,11 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176</f>
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.91036414565826329</v>
+        <v>0.9123287671232877</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
@@ -1191,11 +1191,11 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176</f>
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.88795518207282909</v>
+        <v>0.8904109589041096</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.4649859943977592</v>
+        <v>4.4684931506849317</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -4822,12 +4822,24 @@
         <v>10</v>
       </c>
       <c r="B164" s="12"/>
-      <c r="C164" s="19"/>
-      <c r="D164" s="12"/>
-      <c r="E164" s="12"/>
-      <c r="F164" s="12"/>
-      <c r="G164" s="12"/>
-      <c r="H164" s="56"/>
+      <c r="C164" s="41">
+        <v>8</v>
+      </c>
+      <c r="D164" s="46">
+        <v>5</v>
+      </c>
+      <c r="E164" s="9">
+        <v>8</v>
+      </c>
+      <c r="F164" s="10">
+        <v>0</v>
+      </c>
+      <c r="G164" s="9">
+        <v>8</v>
+      </c>
+      <c r="H164" s="42">
+        <v>8</v>
+      </c>
       <c r="I164" s="36" t="s">
         <v>38</v>
       </c>
@@ -4886,19 +4898,19 @@
         <v>15</v>
       </c>
       <c r="B168" s="11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C168" s="11">
         <f t="shared" ref="C168:H168" si="20">SUM(C163:C167)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D168" s="11">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E168" s="11">
         <f t="shared" si="20"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F168" s="11">
         <f t="shared" si="20"/>
@@ -4906,11 +4918,11 @@
       </c>
       <c r="G168" s="11">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H168" s="11">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I168" s="11"/>
       <c r="J168" s="3"/>

</xml_diff>

<commit_message>
Textures + Uren Registartie
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab 1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\Game-Lab-1.1\Algemeen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jaar 2\Game-Lab-1.1\Game-Lab-1.1\Algemeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -926,23 +926,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E171" sqref="E171 D179"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
-    <col min="3" max="8" width="10.88671875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.109375" customWidth="1"/>
-    <col min="11" max="12" width="22.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="8" width="10.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.140625" customWidth="1"/>
+    <col min="11" max="12" width="22.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>18</v>
       </c>
@@ -977,7 +977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -992,21 +992,21 @@
       <c r="J2" s="1"/>
       <c r="K2" s="12">
         <f>B8+B16+B24+B32+B40+B48+B56+B64+B72+B80+B88+B96+B104+B112+B120+B128+B136+B144+B152+B160+B168+B176+B184</f>
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="L2" s="7">
         <f>C8+C16+C24+C32+C40+C48+C56+C64+C72+C80+C88+C96+C104+C112+C120+C128+C136+C144+C152+C160+C168+C176+C184</f>
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="M2" s="21">
         <f>L2/K2</f>
-        <v>0.73710073710073709</v>
+        <v>0.74216867469879522</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1036,17 +1036,17 @@
       <c r="K3" s="12"/>
       <c r="L3" s="7">
         <f>D8+D16+D24+D32+D40+D48+D56+D64+D72+D80+D88+D96+D104+D112+D120+D128+D136+D144+D152+D160+D168+D176+D184</f>
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="M3" s="21">
         <f>L3/K2</f>
-        <v>0.45454545454545453</v>
+        <v>0.46265060240963857</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1076,17 +1076,17 @@
       <c r="K4" s="12"/>
       <c r="L4" s="7">
         <f>E8+E16+E24+E32+E40+E48+E56+E64+E72+E80+E88+E96+E104+E112+E120+E128+E136+E144+E152+E160+E168+E176+E184</f>
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="M4" s="21">
         <f>L4/K2</f>
-        <v>0.92137592137592139</v>
+        <v>0.92048192771084336</v>
       </c>
       <c r="N4" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1120,13 +1120,13 @@
       </c>
       <c r="M5" s="21">
         <f>L5/K2</f>
-        <v>0.58968058968058967</v>
+        <v>0.57831325301204817</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1154,17 +1154,17 @@
       <c r="K6" s="12"/>
       <c r="L6" s="7">
         <f>G8+G16+G24+G32+G40+G48+G56+G64+G72+G80+G88+G96+G104+G112+G120+G128+G136+G144+G152+G160+G168+G176+G184</f>
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="M6" s="21">
         <f>L6/K2</f>
-        <v>0.91891891891891897</v>
+        <v>0.91807228915662653</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -1194,17 +1194,17 @@
       <c r="K7" s="12"/>
       <c r="L7" s="7">
         <f>H8+H16+H24+H32+H40+H48+H56+H64+H72+H80+H88+H96+H104+H112+H120+H128+H136+H144+H152+H160+H168+H176+H184</f>
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="M7" s="21">
         <f>L7/K2</f>
-        <v>0.90171990171990168</v>
+        <v>0.90361445783132532</v>
       </c>
       <c r="N7" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1239,17 +1239,17 @@
       <c r="J8" s="26"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J9" s="27"/>
       <c r="L9" s="7" t="s">
         <v>75</v>
       </c>
       <c r="M9" s="21">
         <f>SUM(M2:M8)</f>
-        <v>4.5233415233415233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.5253012048192778</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="J12" s="29"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -1446,10 +1446,10 @@
       <c r="J16" s="26"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="J18" s="28"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="J19" s="29"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="J22" s="29"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
@@ -1646,8 +1646,8 @@
       <c r="J24" s="3"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1691,7 +1691,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>13</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
@@ -1846,8 +1846,8 @@
       <c r="J32" s="3"/>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>9</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>11</v>
       </c>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="K38" s="12"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>13</v>
       </c>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="K39" s="12"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>15</v>
       </c>
@@ -2048,8 +2048,8 @@
       <c r="J40" s="3"/>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="12"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="K43" s="12"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>10</v>
       </c>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="K44" s="12"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
@@ -2155,7 +2155,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>13</v>
       </c>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>15</v>
       </c>
@@ -2248,8 +2248,8 @@
       <c r="J48" s="3"/>
       <c r="K48" s="12"/>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>9</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>10</v>
       </c>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="K52" s="12"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>11</v>
       </c>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>12</v>
       </c>
@@ -2384,7 +2384,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>15</v>
       </c>
@@ -2446,8 +2446,8 @@
       <c r="J56" s="3"/>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>24</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>9</v>
       </c>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="K59" s="12"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>10</v>
       </c>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>11</v>
       </c>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="K61" s="12"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>12</v>
       </c>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="K62" s="12"/>
     </row>
-    <row r="63" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>13</v>
       </c>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>15</v>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="J64" s="3"/>
       <c r="K64" s="12"/>
     </row>
-    <row r="65" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="18"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -2659,7 +2659,7 @@
       <c r="I65" s="8"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="J66" s="31"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2689,7 +2689,7 @@
       <c r="J67" s="33"/>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2704,7 +2704,7 @@
       <c r="J68" s="33"/>
       <c r="K68" s="12"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2719,7 +2719,7 @@
       <c r="J69" s="33"/>
       <c r="K69" s="12"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="J70" s="33"/>
       <c r="K70" s="12"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2749,7 +2749,7 @@
       <c r="J71" s="35"/>
       <c r="K71" s="12"/>
     </row>
-    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>15</v>
       </c>
@@ -2784,8 +2784,8 @@
       <c r="J72" s="3"/>
       <c r="K72" s="12"/>
     </row>
-    <row r="73" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
@@ -2800,7 +2800,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="12"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>9</v>
       </c>
@@ -2829,7 +2829,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>10</v>
       </c>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="K76" s="12"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>11</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="K77" s="12"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>12</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="12"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>13</v>
       </c>
@@ -2945,7 +2945,7 @@
       <c r="J79" s="3"/>
       <c r="K79" s="12"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>15</v>
       </c>
@@ -2980,8 +2980,8 @@
       <c r="J80" s="3"/>
       <c r="K80" s="12"/>
     </row>
-    <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>27</v>
       </c>
@@ -2996,7 +2996,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="12"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>9</v>
       </c>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="K83" s="12"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>10</v>
       </c>
@@ -3058,7 +3058,7 @@
       </c>
       <c r="K84" s="12"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>11</v>
       </c>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="K85" s="12"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>12</v>
       </c>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="K86" s="12"/>
     </row>
-    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>13</v>
       </c>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="K87" s="12"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>15</v>
       </c>
@@ -3182,8 +3182,8 @@
       <c r="J88" s="3"/>
       <c r="K88" s="12"/>
     </row>
-    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>28</v>
       </c>
@@ -3198,7 +3198,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>9</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>10</v>
       </c>
@@ -3256,7 +3256,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="12"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>11</v>
       </c>
@@ -3285,7 +3285,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="12"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>12</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="12"/>
     </row>
-    <row r="95" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>13</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="J95" s="3"/>
       <c r="K95" s="12"/>
     </row>
-    <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>15</v>
       </c>
@@ -3374,8 +3374,8 @@
       <c r="J96" s="3"/>
       <c r="K96" s="12"/>
     </row>
-    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>29</v>
       </c>
@@ -3390,7 +3390,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="12"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>9</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="12"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>10</v>
       </c>
@@ -3448,7 +3448,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="12"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>11</v>
       </c>
@@ -3477,7 +3477,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="12"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>12</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="12"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>13</v>
       </c>
@@ -3531,7 +3531,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="12"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>15</v>
       </c>
@@ -3566,8 +3566,8 @@
       <c r="J104" s="3"/>
       <c r="K104" s="12"/>
     </row>
-    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>30</v>
       </c>
@@ -3582,7 +3582,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="12"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>9</v>
       </c>
@@ -3611,7 +3611,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="12"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>10</v>
       </c>
@@ -3640,7 +3640,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="12"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>11</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="12"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>12</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="12"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>13</v>
       </c>
@@ -3723,7 +3723,7 @@
       <c r="J111" s="3"/>
       <c r="K111" s="12"/>
     </row>
-    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>15</v>
       </c>
@@ -3758,8 +3758,8 @@
       <c r="J112" s="3"/>
       <c r="K112" s="12"/>
     </row>
-    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>31</v>
       </c>
@@ -3774,7 +3774,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="12"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>9</v>
       </c>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="K115" s="12"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>10</v>
       </c>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="K116" s="12"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>11</v>
       </c>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="K117" s="12"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>12</v>
       </c>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="K118" s="12"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>13</v>
       </c>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="K119" s="12"/>
     </row>
-    <row r="120" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>15</v>
       </c>
@@ -3959,8 +3959,8 @@
       <c r="J120" s="3"/>
       <c r="K120" s="12"/>
     </row>
-    <row r="121" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>32</v>
       </c>
@@ -3975,7 +3975,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="12"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>9</v>
       </c>
@@ -4004,7 +4004,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="12"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>10</v>
       </c>
@@ -4033,7 +4033,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="12"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>11</v>
       </c>
@@ -4062,7 +4062,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="12"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>12</v>
       </c>
@@ -4089,7 +4089,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="12"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>13</v>
       </c>
@@ -4116,7 +4116,7 @@
       <c r="J127" s="3"/>
       <c r="K127" s="12"/>
     </row>
-    <row r="128" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>15</v>
       </c>
@@ -4151,8 +4151,8 @@
       <c r="J128" s="3"/>
       <c r="K128" s="12"/>
     </row>
-    <row r="129" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>33</v>
       </c>
@@ -4167,7 +4167,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="12"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>9</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="12"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>10</v>
       </c>
@@ -4225,7 +4225,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="12"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>11</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="12"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>12</v>
       </c>
@@ -4281,7 +4281,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="12"/>
     </row>
-    <row r="135" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>13</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="J135" s="3"/>
       <c r="K135" s="12"/>
     </row>
-    <row r="136" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>15</v>
       </c>
@@ -4343,8 +4343,8 @@
       <c r="J136" s="3"/>
       <c r="K136" s="12"/>
     </row>
-    <row r="137" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -4359,7 +4359,7 @@
       <c r="J138" s="31"/>
       <c r="K138" s="12"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -4374,7 +4374,7 @@
       <c r="J139" s="33"/>
       <c r="K139" s="12"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -4389,7 +4389,7 @@
       <c r="J140" s="33"/>
       <c r="K140" s="12"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -4404,7 +4404,7 @@
       <c r="J141" s="33"/>
       <c r="K141" s="12"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>12</v>
       </c>
@@ -4419,7 +4419,7 @@
       <c r="J142" s="33"/>
       <c r="K142" s="12"/>
     </row>
-    <row r="143" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -4434,7 +4434,7 @@
       <c r="J143" s="35"/>
       <c r="K143" s="12"/>
     </row>
-    <row r="144" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>15</v>
       </c>
@@ -4469,8 +4469,8 @@
       <c r="J144" s="3"/>
       <c r="K144" s="12"/>
     </row>
-    <row r="145" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>46</v>
       </c>
@@ -4485,7 +4485,7 @@
       <c r="J146" s="31"/>
       <c r="K146" s="12"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -4500,7 +4500,7 @@
       <c r="J147" s="33"/>
       <c r="K147" s="12"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -4515,7 +4515,7 @@
       <c r="J148" s="33"/>
       <c r="K148" s="12"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -4530,7 +4530,7 @@
       <c r="J149" s="33"/>
       <c r="K149" s="12"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>12</v>
       </c>
@@ -4545,7 +4545,7 @@
       <c r="J150" s="33"/>
       <c r="K150" s="12"/>
     </row>
-    <row r="151" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>13</v>
       </c>
@@ -4560,7 +4560,7 @@
       <c r="J151" s="35"/>
       <c r="K151" s="12"/>
     </row>
-    <row r="152" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6" t="s">
         <v>15</v>
       </c>
@@ -4595,8 +4595,8 @@
       <c r="J152" s="3"/>
       <c r="K152" s="12"/>
     </row>
-    <row r="153" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>35</v>
       </c>
@@ -4611,7 +4611,7 @@
       <c r="J154" s="1"/>
       <c r="K154" s="12"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>9</v>
       </c>
@@ -4640,7 +4640,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="12"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>10</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="12"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>11</v>
       </c>
@@ -4698,7 +4698,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="12"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>12</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="12"/>
     </row>
-    <row r="159" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6" t="s">
         <v>13</v>
       </c>
@@ -4752,7 +4752,7 @@
       <c r="J159" s="3"/>
       <c r="K159" s="12"/>
     </row>
-    <row r="160" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="6" t="s">
         <v>15</v>
       </c>
@@ -4787,8 +4787,8 @@
       <c r="J160" s="3"/>
       <c r="K160" s="12"/>
     </row>
-    <row r="161" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>36</v>
       </c>
@@ -4803,7 +4803,7 @@
       <c r="J162" s="1"/>
       <c r="K162" s="12"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>9</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="12"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>10</v>
       </c>
@@ -4861,7 +4861,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="12"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>11</v>
       </c>
@@ -4890,7 +4890,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="12"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>12</v>
       </c>
@@ -4917,7 +4917,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="12"/>
     </row>
-    <row r="167" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="6" t="s">
         <v>13</v>
       </c>
@@ -4944,7 +4944,7 @@
       <c r="J167" s="3"/>
       <c r="K167" s="12"/>
     </row>
-    <row r="168" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="6" t="s">
         <v>15</v>
       </c>
@@ -4979,8 +4979,8 @@
       <c r="J168" s="3"/>
       <c r="K168" s="12"/>
     </row>
-    <row r="169" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>37</v>
       </c>
@@ -4995,7 +4995,7 @@
       <c r="J170" s="1"/>
       <c r="K170" s="12"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>9</v>
       </c>
@@ -5024,7 +5024,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="12"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>10</v>
       </c>
@@ -5053,7 +5053,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="12"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>11</v>
       </c>
@@ -5082,7 +5082,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="12"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>12</v>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="12"/>
     </row>
-    <row r="175" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>13</v>
       </c>
@@ -5136,7 +5136,7 @@
       <c r="J175" s="3"/>
       <c r="K175" s="12"/>
     </row>
-    <row r="176" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
         <v>15</v>
       </c>
@@ -5171,8 +5171,8 @@
       <c r="J176" s="3"/>
       <c r="K176" s="12"/>
     </row>
-    <row r="177" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>76</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="I178" s="47"/>
       <c r="J178" s="1"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>9</v>
       </c>
@@ -5214,23 +5214,35 @@
       </c>
       <c r="J179" s="2"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B180" s="12"/>
-      <c r="C180" s="19"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
-      <c r="G180" s="12"/>
-      <c r="H180" s="56"/>
+      <c r="C180" s="41">
+        <v>8</v>
+      </c>
+      <c r="D180" s="46">
+        <v>7</v>
+      </c>
+      <c r="E180" s="46">
+        <v>7</v>
+      </c>
+      <c r="F180" s="10">
+        <v>0</v>
+      </c>
+      <c r="G180" s="46">
+        <v>7</v>
+      </c>
+      <c r="H180" s="42">
+        <v>8</v>
+      </c>
       <c r="I180" s="36" t="s">
         <v>38</v>
       </c>
       <c r="J180" s="2"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>11</v>
       </c>
@@ -5246,7 +5258,7 @@
       </c>
       <c r="J181" s="2"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>12</v>
       </c>
@@ -5260,7 +5272,7 @@
       <c r="I182" s="38"/>
       <c r="J182" s="2"/>
     </row>
-    <row r="183" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>13</v>
       </c>
@@ -5274,24 +5286,24 @@
       <c r="I183" s="39"/>
       <c r="J183" s="3"/>
     </row>
-    <row r="184" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B184" s="11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C184" s="11">
         <f t="shared" ref="C184:H184" si="22">SUM(C179:C183)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D184" s="11">
         <f t="shared" si="22"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E184" s="11">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F184" s="11">
         <f t="shared" si="22"/>
@@ -5299,11 +5311,11 @@
       </c>
       <c r="G184" s="11">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H184" s="11">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I184" s="11"/>
       <c r="J184" s="3"/>

</xml_diff>